<commit_message>
Added documentation to code. Added American to UK English translation to improve consistency. Redid suggesting verbs for failed cases. Renamed mapped verb output files.
</commit_message>
<xml_diff>
--- a/outputs/failed_lo_mappings.xlsx
+++ b/outputs/failed_lo_mappings.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mappings" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Suggested Verbs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F118"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +459,11 @@
           <t>Verbs Identified</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Suggested Verbs</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -486,6 +490,11 @@
           <t>[('discern', 'Verb not mapped'), ('propose', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>[('change', 'Applying'), ('justify', 'Creating'), ('give', 'Understanding'), ('apply', 'Applying'), ('describe', 'Understanding')]</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -508,12 +517,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>[('identify', 'Understanding'), ('provide', 'Verb not mapped'), ('analyse', 'Analysing'), ('use', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[('describe', 'Understanding'), ('apply', 'Applying'), ('define', 'Remembering'), ('generate', 'Creating'), ('organise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -546,6 +560,11 @@
           <t>[('identify', 'Understanding'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[('perform', 'Creating'), ('identify', 'Understanding'), ('adopt', 'Evaluating'), ('support', 'Evaluating'), ('devise', 'Evaluating')]</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -576,6 +595,11 @@
           <t>[('determine', 'Verb not mapped'), ('include', 'Verb not mapped'), ('embody', 'Verb not mapped'), ('propose', 'Verb not mapped'), ('use', 'Applying')]</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>[('describe', 'Understanding'), ('apply', 'Applying'), ('define', 'Remembering'), ('generate', 'Creating'), ('organise', 'Evaluating')]</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -606,6 +630,11 @@
           <t>[('identify', 'Unistructural'), ('select', 'Multistructural'), ('derive', 'Relational')]</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>[('summarise', 'Relational'), ('differentiate', 'Relational'), ('mitigate', 'Extended Abstract'), ('generate', 'Extended Abstract'), ('describe', 'Multistructural')]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -636,6 +665,11 @@
           <t>[('discuss', 'Relational'), ('write', 'Unistructural')]</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>[('sequence', 'Multistructural'), ('generate', 'Extended Abstract'), ('describe', 'Multistructural'), ('summarise', 'Relational'), ('differentiate', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -666,6 +700,11 @@
           <t>[('engage', 'Extended Abstract')]</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>[('review', 'Extended Abstract'), ('discuss', 'Relational'), ('address', 'Relational'), ('demonstrate', 'Extended Abstract'), ('value', 'Extended Abstract')]</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -696,6 +735,11 @@
           <t>[('discuss', 'Relational'), ('integrate', 'Extended Abstract')]</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[('mitigate', 'Extended Abstract'), ('generate', 'Extended Abstract'), ('address', 'Relational'), ('prove', 'Relational'), ('create', 'Extended Abstract')]</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -726,6 +770,11 @@
           <t>[('define', 'Remembering'), ('use', 'Applying'), ('discern', 'Verb not mapped'), ('solve', 'Applying'), ('decompose', 'Verb not mapped'), ('use', 'Applying'), ('describe', 'Understanding')]</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>[('define', 'Remembering'), ('justify', 'Creating'), ('change', 'Applying'), ('rate', 'Evaluating'), ('characterise', 'Understanding')]</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -756,6 +805,11 @@
           <t>[('select', 'Evaluating'), ('solve', 'Applying'), ('contain', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>[('produce', 'Creating'), ('state', 'Remembering'), ('back', 'Applying'), ('act', 'Applying'), ('perform', 'Creating')]</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -786,6 +840,11 @@
           <t>[('propose', 'Multistructural'), ('give', 'Verb not mapped'), ('evaluate', 'Extended Abstract')]</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>[('prove', 'Relational'), ('contrast', 'Relational'), ('mitigate', 'Extended Abstract'), ('address', 'Relational'), ('compare', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -816,6 +875,11 @@
           <t>[('identify', 'Unistructural'), ('reflect', 'Extended Abstract'), ('contribute', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>[('reflect', 'Extended Abstract'), ('conduct', 'Relational'), ('evaluate', 'Extended Abstract'), ('relate', 'Relational'), ('use', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -842,6 +906,11 @@
           <t>[('determine', 'Verb not mapped'), ('inform', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>[('act', 'Applying'), ('summarise', 'Understanding'), ('rate', 'Evaluating'), ('change', 'Applying'), ('generate', 'Creating')]</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -872,6 +941,11 @@
           <t>[('determine', 'Verb not mapped'), ('involve', 'Verb not mapped'), ('use', 'Applying'), ('solve', 'Applying')]</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>[('design', 'Creating'), ('justify', 'Creating'), ('apply', 'Applying'), ('change', 'Applying'), ('develop', 'Creating')]</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -902,6 +976,11 @@
           <t>[('identify', 'Unistructural'), ('develop', 'Verb not mapped'), ('validate', 'Verb not mapped'), ('convey', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>[('summarise', 'Relational'), ('compare', 'Relational'), ('synthesise', 'Extended Abstract'), ('generate', 'Extended Abstract'), ('organise', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -932,6 +1011,11 @@
           <t>[('identify', 'Unistructural'), ('reflect', 'Extended Abstract'), ('contribute', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>[('reflect', 'Extended Abstract'), ('conduct', 'Relational'), ('evaluate', 'Extended Abstract'), ('relate', 'Relational'), ('use', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -958,6 +1042,11 @@
           <t>[('determine', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>[('perform', 'Creating'), ('identify', 'Understanding'), ('adopt', 'Evaluating'), ('support', 'Evaluating'), ('devise', 'Evaluating')]</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -988,6 +1077,11 @@
           <t>[('evaluate', 'Extended Abstract')]</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>[('prove', 'Relational'), ('contrast', 'Relational'), ('mitigate', 'Extended Abstract'), ('address', 'Relational'), ('compare', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1018,6 +1112,11 @@
           <t>[('analyse', 'Relational'), ('determine', 'Multistructural')]</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>[('report', 'Multistructural'), ('identify', 'Unistructural'), ('compare', 'Relational'), ('define', 'Multistructural'), ('prove', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1048,6 +1147,11 @@
           <t>[('work', 'Verb not mapped'), ('analyse', 'Relational'), ('write', 'Unistructural')]</t>
         </is>
       </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>[('sequence', 'Multistructural'), ('generate', 'Extended Abstract'), ('describe', 'Multistructural'), ('summarise', 'Relational'), ('differentiate', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1078,6 +1182,11 @@
           <t>[('apply', 'Applying'), ('orient', 'Verb not mapped'), ('design', 'Creating'), ('use', 'Applying')]</t>
         </is>
       </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>[('describe', 'Understanding'), ('apply', 'Applying'), ('define', 'Remembering'), ('generate', 'Creating'), ('organise', 'Evaluating')]</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1108,6 +1217,11 @@
           <t>[('prove', 'Evaluating'), ('analyse', 'Analysing')]</t>
         </is>
       </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>[('implement', 'Applying'), ('perform', 'Creating'), ('evaluate', 'Evaluating'), ('compare', 'Understanding'), ('describe', 'Understanding')]</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1138,6 +1252,11 @@
           <t>[('compare', 'Understanding'), ('contrast', 'Analysing'), ('use', 'Applying')]</t>
         </is>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>[('describe', 'Understanding'), ('apply', 'Applying'), ('define', 'Remembering'), ('generate', 'Creating'), ('organise', 'Evaluating')]</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1164,6 +1283,11 @@
           <t>[('develop', 'Verb not mapped'), ('implement', 'Verb not mapped'), ('solve', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>[('design', 'Extended Abstract'), ('propose', 'Multistructural'), ('justify', 'Extended Abstract'), ('apply', 'Relational'), ('select', 'Multistructural')]</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1194,6 +1318,11 @@
           <t>[('identify', 'Unistructural'), ('include', 'Verb not mapped'), ('select', 'Multistructural'), ('give', 'Verb not mapped'), ('achieve', 'Verb not mapped'), ('document', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>[('generate', 'Extended Abstract'), ('sequence', 'Multistructural'), ('address', 'Relational'), ('mitigate', 'Extended Abstract'), ('organise', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1224,6 +1353,11 @@
           <t>[('perform', 'Verb not mapped'), ('use', 'Relational'), ('base', 'Verb not mapped'), ('base', 'Verb not mapped'), ('utilise', 'Verb not mapped'), ('automate', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>[('identify', 'Unistructural'), ('address', 'Relational'), ('integrate', 'Extended Abstract'), ('report', 'Multistructural'), ('mitigate', 'Extended Abstract')]</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1254,6 +1388,11 @@
           <t>[('perform', 'Verb not mapped'), ('use', 'Relational'), ('trace', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>[('address', 'Relational'), ('generate', 'Extended Abstract'), ('sequence', 'Multistructural'), ('mitigate', 'Extended Abstract'), ('contrast', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1284,6 +1423,11 @@
           <t>[('select', 'Multistructural'), ('collect', 'Verb not mapped'), ('include', 'Verb not mapped'), ('analyse', 'Relational'), ('make', 'Verb not mapped'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Extended Abstract'), ('differentiate', 'Relational'), ('derive', 'Relational'), ('conduct', 'Relational'), ('function', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1314,6 +1458,11 @@
           <t>[('explain', 'Understanding'), ('analyse', 'Analysing')]</t>
         </is>
       </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>[('implement', 'Applying'), ('perform', 'Creating'), ('evaluate', 'Evaluating'), ('compare', 'Understanding'), ('describe', 'Understanding')]</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1344,6 +1493,11 @@
           <t>[('explain', 'Understanding'), ('analyse', 'Analysing')]</t>
         </is>
       </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>[('implement', 'Applying'), ('perform', 'Creating'), ('evaluate', 'Evaluating'), ('compare', 'Understanding'), ('describe', 'Understanding')]</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1374,6 +1528,11 @@
           <t>[('model', 'Verb not mapped'), ('design', 'Organisation'), ('use', 'Receiving')]</t>
         </is>
       </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>[('describe', 'Receiving'), ('guide', 'Valuing'), ('organise', 'Organisation'), ('allow', 'Responding'), ('justify', 'Valuing')]</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1404,6 +1563,11 @@
           <t>[('analyse', 'Analysing'), ('design', 'Creating'), ('refactor', 'Verb not mapped'), ('take', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>[('make', 'Creating'), ('discuss', 'Understanding'), ('perform', 'Creating'), ('generate', 'Creating'), ('produce', 'Creating')]</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1430,6 +1594,11 @@
           <t>[('take', 'Verb not mapped'), ('develop', 'Verb not mapped'), ('follow', 'Verb not mapped'), ('orient', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>[('describe', 'Multistructural'), ('generate', 'Extended Abstract'), ('mitigate', 'Extended Abstract'), ('discuss', 'Relational'), ('sequence', 'Multistructural')]</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1460,6 +1629,11 @@
           <t>[('select', 'Receiving'), ('use', 'Receiving'), ('incremente', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>[('allow', 'Responding'), ('choose', 'Receiving'), ('relay', 'Responding'), ('respond', 'Responding'), ('change', 'Characterisation')]</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1490,6 +1664,11 @@
           <t>[('evaluate', 'Extended Abstract'), ('apply', 'Relational'), ('design', 'Extended Abstract')]</t>
         </is>
       </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>[('design', 'Extended Abstract'), ('apply', 'Relational'), ('select', 'Multistructural'), ('propose', 'Multistructural'), ('review', 'Extended Abstract')]</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1520,6 +1699,11 @@
           <t>[('describe', 'Multistructural'), ('base', 'Verb not mapped'), ('apply', 'Relational'), ('achieve', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>[('review', 'Extended Abstract'), ('generate', 'Extended Abstract'), ('engage', 'Extended Abstract'), ('manage', 'Relational'), ('identify', 'Unistructural')]</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1550,6 +1734,11 @@
           <t>[('apply', 'Relational'), ('engage', 'Extended Abstract'), ('determine', 'Multistructural')]</t>
         </is>
       </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>[('report', 'Multistructural'), ('identify', 'Unistructural'), ('compare', 'Relational'), ('define', 'Multistructural'), ('prove', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1580,6 +1769,11 @@
           <t>[('plan', 'Extended Abstract'), ('manage', 'Relational')]</t>
         </is>
       </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>[('organise', 'Relational'), ('plan', 'Extended Abstract'), ('manage', 'Relational'), ('describe', 'Multistructural'), ('identify', 'Unistructural')]</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1610,6 +1804,11 @@
           <t>[('compare', 'Understanding'), ('analyse', 'Analysing'), ('determine', 'Verb not mapped'), ('require', 'Verb not mapped'), ('support', 'Evaluating')]</t>
         </is>
       </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>[('make', 'Creating'), ('characterise', 'Understanding'), ('generate', 'Creating'), ('report', 'Understanding'), ('rate', 'Evaluating')]</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1640,6 +1839,11 @@
           <t>[('deliberate', 'Extended Abstract'), ('occur', 'Verb not mapped'), ('identify', 'Unistructural'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>[('conduct', 'Relational'), ('evaluate', 'Extended Abstract'), ('differentiate', 'Relational'), ('derive', 'Relational'), ('function', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1666,6 +1870,11 @@
           <t>[('develop', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>[('select', 'Multistructural'), ('apply', 'Relational'), ('design', 'Extended Abstract'), ('differentiate', 'Relational'), ('use', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1692,6 +1901,11 @@
           <t>[('implement', 'Verb not mapped'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Extended Abstract'), ('differentiate', 'Relational'), ('derive', 'Relational'), ('function', 'Relational'), ('write', 'Unistructural')]</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1722,6 +1936,11 @@
           <t>[('manage', 'Organisation'), ('meet', 'Receiving'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>[('perform', 'Characterisation'), ('identify', 'Receiving'), ('adopt', 'Valuing'), ('support', 'Valuing'), ('allow', 'Responding')]</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1748,6 +1967,11 @@
           <t>[('develop', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>[('select', 'Multistructural'), ('apply', 'Relational'), ('design', 'Extended Abstract'), ('differentiate', 'Relational'), ('use', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1778,6 +2002,11 @@
           <t>[('analyse', 'Analysing'), ('apply', 'Applying')]</t>
         </is>
       </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>[('justify', 'Creating'), ('summarise', 'Understanding'), ('back', 'Applying'), ('describe', 'Understanding'), ('generate', 'Creating')]</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1808,6 +2037,11 @@
           <t>[('analyse', 'Analysing'), ('implement', 'Applying'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>[('perform', 'Creating'), ('identify', 'Understanding'), ('adopt', 'Evaluating'), ('support', 'Evaluating'), ('devise', 'Evaluating')]</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1838,6 +2072,11 @@
           <t>[('analyse', 'Analysing'), ('implement', 'Applying'), ('base', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>[('perform', 'Creating'), ('identify', 'Understanding'), ('adopt', 'Evaluating'), ('support', 'Evaluating'), ('devise', 'Evaluating')]</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1868,6 +2107,11 @@
           <t>[('implement', 'Verb not mapped'), ('evaluate', 'Extended Abstract'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Extended Abstract'), ('differentiate', 'Relational'), ('derive', 'Relational'), ('function', 'Relational'), ('write', 'Unistructural')]</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1898,6 +2142,11 @@
           <t>[('design', 'Extended Abstract'), ('implement', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>[('function', 'Relational'), ('evaluate', 'Extended Abstract'), ('analyse', 'Relational'), ('derive', 'Relational'), ('apply', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1928,6 +2177,11 @@
           <t>[('select', 'Multistructural'), ('use', 'Relational'), ('manage', 'Relational'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>[('identify', 'Unistructural'), ('address', 'Relational'), ('integrate', 'Extended Abstract'), ('report', 'Multistructural'), ('mitigate', 'Extended Abstract')]</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1950,12 +2204,17 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Unistructural</t>
+          <t>Extended Abstract</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
           <t>[('identify', 'Unistructural'), ('include', 'Verb not mapped'), ('devise', 'Verb not mapped'), ('adopt', 'Verb not mapped'), ('monitor', 'Verb not mapped'), ('mitigate', 'Extended Abstract')]</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>[('mitigate', 'Extended Abstract'), ('address', 'Relational'), ('integrate', 'Extended Abstract'), ('generate', 'Extended Abstract'), ('characterise', 'Relational')]</t>
         </is>
       </c>
     </row>
@@ -1988,6 +2247,11 @@
           <t>[('choose', 'Verb not mapped'), ('follow', 'Verb not mapped'), ('justify', 'Extended Abstract')]</t>
         </is>
       </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>[('describe', 'Multistructural'), ('generate', 'Extended Abstract'), ('derive', 'Relational'), ('apply', 'Relational'), ('appreciate', 'Relational')]</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2014,70 +2278,81 @@
           <t>[('include', 'Verb not mapped'), ('ensure', 'Verb not mapped'), ('communicate', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>[('justify', 'Extended Abstract'), ('engage', 'Extended Abstract'), ('report', 'Multistructural'), ('address', 'Relational'), ('generate', 'Extended Abstract')]</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Produce internal documentation of a sufficient quality to support project development activities (including specification, analysis, design, testing) and address relevant security and other risks</t>
+          <t>Communicate effectively with a diverse range of project stakeholders, including clients, end users, and supervisors</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>SOLO</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Creating</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Evaluating</t>
-        </is>
-      </c>
+          <t>Multistructural</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[('produce', 'Creating'), ('support', 'Evaluating'), ('include', 'Verb not mapped'), ('address', 'Verb not mapped')]</t>
+          <t>[('communicate', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>[('identify', 'Unistructural'), ('address', 'Relational'), ('integrate', 'Extended Abstract'), ('report', 'Multistructural'), ('mitigate', 'Extended Abstract')]</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Communicate effectively with a diverse range of project stakeholders, including clients, end users, and supervisors</t>
+          <t>Verify systematically that internal and external project deliverables meet agreed quality standards, such as functionality, security and usability</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Multistructural</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>[('communicate', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+          <t>[('verify', 'Verb not mapped'), ('meet', 'Verb not mapped'), ('agree', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>[('generate', 'Creating'), ('rate', 'Evaluating'), ('perform', 'Creating'), ('prove', 'Evaluating'), ('make', 'Creating')]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Verify systematically that internal and external project deliverables meet agreed quality standards, such as functionality, security and usability</t>
+          <t>Research relevant and reliable literature to evaluate the state of the field.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2090,50 +2365,64 @@
           <t>Evaluating</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>[('verify', 'Verb not mapped'), ('meet', 'Verb not mapped'), ('agree', 'Verb not mapped')]</t>
+          <t>[('research', 'Analysing'), ('evaluate', 'Evaluating')]</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>[('perform', 'Creating'), ('state', 'Remembering'), ('back', 'Applying'), ('prove', 'Evaluating'), ('contrast', 'Analysing')]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Research relevant and reliable literature to evaluate the state of the field.</t>
+          <t>Analyse a problem and evaluate the potential of a solution or experiment.</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>SOLO</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Evaluating</t>
+          <t xml:space="preserve">Extended abstract </t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Analysing</t>
+          <t>Relational</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>[('research', 'Analysing'), ('evaluate', 'Evaluating')]</t>
+          <t>[('analyse', 'Relational'), ('evaluate', 'Extended Abstract')]</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>[('prove', 'Relational'), ('contrast', 'Relational'), ('mitigate', 'Extended Abstract'), ('address', 'Relational'), ('compare', 'Relational')]</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Analyse a problem and evaluate the potential of a solution or experiment.</t>
+          <t>Appraise a complex engineering problem and investigate it using appropriate research methods and techniques.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2153,223 +2442,263 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>[('analyse', 'Relational'), ('evaluate', 'Extended Abstract')]</t>
+          <t>[('appraise', 'Extended Abstract'), ('investigate', 'Verb not mapped'), ('use', 'Relational')]</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>[('describe', 'Multistructural'), ('apply', 'Relational'), ('define', 'Multistructural'), ('reduce', 'Relational'), ('derive', 'Relational')]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Appraise a complex engineering problem and investigate it using appropriate research methods and techniques.</t>
+          <t>Integrate foundational and discipline-specific knowledge to solve complex open-ended problems.</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Extended abstract </t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>[('appraise', 'Extended Abstract'), ('investigate', 'Verb not mapped'), ('use', 'Relational')]</t>
+          <t>[('integrate', 'Evaluating'), ('solve', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>[('design', 'Creating'), ('review', 'Remembering'), ('justify', 'Creating'), ('apply', 'Applying'), ('change', 'Applying')]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Integrate foundational and discipline-specific knowledge to solve complex open-ended problems.</t>
+          <t>Plan the scope and requirements of a research project or experiment, responding to changing requirements and potential interdisciplinary inputs.</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>SOLO</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Organisation/Characterisation</t>
+          <t>Extended abstract</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Relational</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[('integrate', 'Organisation'), ('solve', 'Characterisation')]</t>
+          <t>[('plan', 'Extended Abstract'), ('respond', 'Verb not mapped'), ('change', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>[('generate', 'Extended Abstract'), ('justify', 'Extended Abstract'), ('address', 'Relational'), ('describe', 'Multistructural'), ('summarise', 'Relational')]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Plan the scope and requirements of a research project or experiment, responding to changing requirements and potential interdisciplinary inputs.</t>
+          <t>Generate research and technical outputs by applying appropriate techniques, resources and modern engineering tools to a complex open-ended engineering problem.</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>SOLO</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Extended abstract</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Responding</t>
+          <t>Relational</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>[('plan', 'Organisation'), ('respond', 'Responding'), ('change', 'Characterisation')]</t>
+          <t>[('generate', 'Extended Abstract'), ('apply', 'Relational')]</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>[('justify', 'Extended Abstract'), ('summarise', 'Relational'), ('describe', 'Multistructural'), ('generate', 'Extended Abstract'), ('apply', 'Relational')]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Generate research and technical outputs by applying appropriate techniques, resources and modern engineering tools to a complex open-ended engineering problem.</t>
+          <t>Demonstrate consideration of the ethics and norms which guide engineering practice, including professionalism, innovation and creativity.</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Extended abstract</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>[('generate', 'Extended Abstract'), ('apply', 'Relational')]</t>
+          <t>[('demonstrate', 'Valuing'), ('guide', 'Valuing'), ('include', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>[('perform', 'Characterisation'), ('identify', 'Receiving'), ('adopt', 'Valuing'), ('support', 'Valuing'), ('allow', 'Responding')]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Demonstrate consideration of the ethics and norms which guide engineering practice, including professionalism, innovation and creativity.</t>
+          <t>Assess the social, health, safety, legal, cultural, commercial and political impacts of the identified project, as appropriate.</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>SOLO</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Responding</t>
+          <t>Extended abstract</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Valuing</t>
+          <t>Unistructural</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Valuing'), ('guide', 'Valuing'), ('include', 'Verb not mapped')]</t>
+          <t>[('assess', 'Extended Abstract'), ('identify', 'Unistructural')]</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>[('address', 'Relational'), ('synthesise', 'Extended Abstract'), ('determine', 'Multistructural'), ('discuss', 'Relational'), ('mitigate', 'Extended Abstract')]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Assess the social, health, safety, legal, cultural, commercial and political impacts of the identified project, as appropriate.</t>
+          <t>Synthesise the progress and outputs of your project through professional engineering reports and presentations to a range of audiences including the community and industry.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Extended abstract</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>Unistructural</t>
-        </is>
-      </c>
+          <t>Creating</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>[('assess', 'Extended Abstract'), ('identify', 'Unistructural')]</t>
+          <t>[('synthesise', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>[('perform', 'Creating'), ('identify', 'Understanding'), ('adopt', 'Evaluating'), ('support', 'Evaluating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Synthesise the progress and outputs of your project through professional engineering reports and presentations to a range of audiences including the community and industry.</t>
+          <t>Engage with project collaborators to achieve research outcomes using effective self and/or team management, review and improvement practices. (Applicable to the Clayton-based course)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>SOLO</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Organization</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr"/>
+          <t>Extended abstract</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Relational</t>
+        </is>
+      </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>[('synthesise', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+          <t>[('engage', 'Extended Abstract'), ('achieve', 'Verb not mapped'), ('use', 'Relational'), ('base', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Extended Abstract'), ('differentiate', 'Relational'), ('derive', 'Relational'), ('function', 'Relational'), ('write', 'Unistructural')]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Engage with project collaborators to achieve research outcomes using effective self and/or team management, review and improvement practices. (Applicable to the Clayton-based course)</t>
+          <t>identify and explain big data concepts and technologies;</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2379,27 +2708,32 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Extended abstract</t>
+          <t>Relational</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Unistructural</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>[('engage', 'Extended Abstract'), ('achieve', 'Verb not mapped'), ('use', 'Relational'), ('base', 'Verb not mapped')]</t>
+          <t>[('identify', 'Unistructural'), ('explain', 'Relational')]</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>[('characterise', 'Relational'), ('describe', 'Multistructural'), ('sequence', 'Multistructural'), ('mitigate', 'Extended Abstract'), ('discuss', 'Relational')]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>identify and explain big data concepts and technologies;</t>
+          <t>write and interpret parallel database processing algorithms and methods;</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2419,17 +2753,22 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>[('identify', 'Unistructural'), ('explain', 'Relational')]</t>
+          <t>[('write', 'Unistructural'), ('interpret', 'Relational')]</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>[('summarise', 'Relational'), ('compute', 'Relational'), ('generate', 'Extended Abstract'), ('reduce', 'Relational'), ('write', 'Unistructural')]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>write and interpret parallel database processing algorithms and methods;</t>
+          <t>use and evaluate streaming methods in big data processing;</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2439,57 +2778,67 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
+          <t>Extended abstract</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
           <t>Relational</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>Unistructural</t>
-        </is>
-      </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>[('write', 'Unistructural'), ('interpret', 'Relational')]</t>
+          <t>[('use', 'Relational'), ('evaluate', 'Extended Abstract')]</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>[('prove', 'Relational'), ('contrast', 'Relational'), ('mitigate', 'Extended Abstract'), ('address', 'Relational'), ('compare', 'Relational')]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>use and evaluate streaming methods in big data processing;</t>
+          <t>use big data streaming technologies.</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Extended abstract</t>
+          <t>Recieving</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Receiving</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>[('use', 'Relational'), ('evaluate', 'Extended Abstract')]</t>
+          <t>[('use', 'Receiving'), ('stream', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>[('describe', 'Receiving'), ('guide', 'Valuing'), ('organise', 'Organisation'), ('allow', 'Responding'), ('justify', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>use big data streaming technologies.</t>
+          <t>be responsible and effective global citizens who engage in an internationalised world by being able to demonstrate cross cultural competencies and empathy whilst acting ethically and sustainably</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2499,27 +2848,32 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Recieving</t>
+          <t>Characterisation</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Receiving</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>[('use', 'Receiving'), ('stream', 'Verb not mapped')]</t>
+          <t>[('engage', 'Verb not mapped'), ('demonstrate', 'Valuing'), ('act', 'Characterisation')]</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>[('allow', 'Responding'), ('guide', 'Valuing'), ('consider', 'Organisation'), ('object', 'Characterisation'), ('compare', 'Organisation')]</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>be responsible and effective global citizens who engage in an internationalised world by being able to demonstrate cross cultural competencies and empathy whilst acting ethically and sustainably</t>
+          <t>demonstrate broad knowledge and technical capabilities driven by an entrepreneurial mindset across a variety of domains including but not limited to the business, professional and public policy communities that we serve</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2529,17 +2883,22 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
+          <t>Valuing</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
           <t>Characterisation</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Valuing</t>
-        </is>
-      </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>[('engage', 'Verb not mapped'), ('demonstrate', 'Valuing'), ('act', 'Characterisation')]</t>
+          <t>[('demonstrate', 'Valuing'), ('drive', 'Verb not mapped'), ('include', 'Verb not mapped'), ('limit', 'Verb not mapped'), ('serve', 'Characterisation')]</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>[('allow', 'Responding'), ('study', 'Valuing'), ('delay', 'Valuing'), ('organise', 'Organisation'), ('consider', 'Organisation')]</t>
         </is>
       </c>
     </row>
@@ -2572,6 +2931,11 @@
           <t>[('understand', 'Verb not mapped'), ('test', 'Organisation'), ('relate', 'Organisation')]</t>
         </is>
       </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>[('change', 'Characterisation'), ('establish', 'Organisation'), ('investigate', 'Organisation'), ('delay', 'Valuing'), ('allow', 'Responding')]</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2602,6 +2966,11 @@
           <t>[('develop', 'Verb not mapped'), ('manage', 'Organisation'), ('work', 'Valuing'), ('start', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>[('relay', 'Responding'), ('allow', 'Responding'), ('study', 'Valuing'), ('organise', 'Organisation'), ('choose', 'Receiving')]</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2632,6 +3001,11 @@
           <t>[('consider', 'Organisation'), ('create', 'Verb not mapped'), ('challenge', 'Characterisation'), ('integrate', 'Organisation'), ('accommodate', 'Verb not mapped'), ('differ', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>[('challenge', 'Characterisation'), ('allow', 'Responding'), ('consider', 'Organisation'), ('organise', 'Organisation'), ('act', 'Characterisation')]</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2649,13 +3023,18 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr">
         <is>
           <t>[('reflect', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>[('contribute', 'Valuing'), ('lead', 'Organisation'), ('identify', 'Receiving'), ('choose', 'Receiving'), ('relay', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -2688,6 +3067,11 @@
           <t>[('describe', 'Receiving')]</t>
         </is>
       </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>[('allow', 'Responding'), ('relay', 'Responding'), ('follow', 'Receiving'), ('guide', 'Valuing'), ('justify', 'Valuing')]</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2705,13 +3089,18 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr">
         <is>
           <t>[('determine', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>[('report', 'Valuing'), ('identify', 'Receiving'), ('compare', 'Organisation'), ('respond', 'Responding'), ('agree', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -2740,6 +3129,11 @@
           <t>[('comprehend', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>[('delay', 'Valuing'), ('guide', 'Valuing'), ('respond', 'Responding'), ('act', 'Characterisation'), ('lead', 'Organisation')]</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2767,6 +3161,11 @@
           <t>[('assess', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>[('agree', 'Responding'), ('discuss', 'Responding'), ('study', 'Valuing'), ('lead', 'Organisation'), ('adopt', 'Valuing')]</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2797,6 +3196,11 @@
           <t>[('describe', 'Receiving')]</t>
         </is>
       </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>[('allow', 'Responding'), ('relay', 'Responding'), ('follow', 'Receiving'), ('guide', 'Valuing'), ('justify', 'Valuing')]</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2828,6 +3232,11 @@
           <t>[('apply', 'Verb not mapped'), ('learn', 'Verb not mapped'), ('design', 'Organisation')]</t>
         </is>
       </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>[('select', 'Receiving'), ('solve', 'Characterisation'), ('propose', 'Characterisation'), ('justify', 'Valuing'), ('describe', 'Receiving')]</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2858,6 +3267,11 @@
           <t>[('integrate', 'Organisation'), ('evaluate', 'Valuing'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>[('perform', 'Characterisation'), ('identify', 'Receiving'), ('adopt', 'Valuing'), ('support', 'Valuing'), ('allow', 'Responding')]</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2884,14 +3298,19 @@
           <t>[('apply', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>[('perform', 'Characterisation'), ('identify', 'Receiving'), ('adopt', 'Valuing'), ('support', 'Valuing'), ('allow', 'Responding')]</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Identify the elements of the project life cycle, including plan, control, and organise and allocate resources.</t>
+          <t>Evaluate and apply the basic tools and techniques to plan, organise and manage a project.</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2901,27 +3320,32 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
+          <t>Valuing</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
           <t>Organisation</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>Receiving</t>
-        </is>
-      </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>[('identify', 'Receiving'), ('include', 'Verb not mapped'), ('plan', 'Organisation'), ('control', 'Verb not mapped'), ('organise', 'Verb not mapped'), ('allocate', 'Verb not mapped')]</t>
+          <t>[('evaluate', 'Valuing'), ('apply', 'Verb not mapped'), ('plan', 'Organisation'), ('organise', 'Organisation'), ('manage', 'Organisation')]</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>[('manage', 'Organisation'), ('organise', 'Organisation'), ('follow', 'Receiving'), ('work', 'Valuing'), ('support', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Evaluate and apply the basic tools and techniques to plan, organise and manage a project.</t>
+          <t>Identify strategic constraints in managing the scope, time, cost and quality components.</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2931,27 +3355,32 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Valuing</t>
+          <t>Recieving</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Receiving</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>[('evaluate', 'Valuing'), ('apply', 'Verb not mapped'), ('plan', 'Organisation'), ('organise', 'Verb not mapped'), ('manage', 'Organisation')]</t>
+          <t>[('identify', 'Receiving'), ('manage', 'Organisation')]</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>[('organise', 'Organisation'), ('follow', 'Receiving'), ('work', 'Valuing'), ('support', 'Valuing'), ('plan', 'Organisation')]</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Identify strategic constraints in managing the scope, time, cost and quality components.</t>
+          <t>Discuss professional responsibility, occupational health and safety and ethical conduct.</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2961,27 +3390,32 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Recieving</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Receiving</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>[('identify', 'Receiving'), ('manage', 'Organisation')]</t>
+          <t>[('discuss', 'Responding')]</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>[('allow', 'Responding'), ('respond', 'Responding'), ('relay', 'Responding'), ('lead', 'Organisation'), ('establish', 'Organisation')]</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Discuss professional responsibility, occupational health and safety and ethical conduct.</t>
+          <t>Describe the purpose of enterprise architectures and the underlying principles of their design;</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2991,27 +3425,32 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Valuing</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Responding</t>
+          <t>Receiving</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>[('discuss', 'Responding')]</t>
+          <t>[('describe', 'Receiving'), ('underlie', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>[('perform', 'Characterisation'), ('allow', 'Responding'), ('agree', 'Responding'), ('consider', 'Organisation'), ('describe', 'Receiving')]</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Describe the purpose of enterprise architectures and the underlying principles of their design;</t>
+          <t>Describe into the need for sound data, information and technology governance strategies;</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3021,7 +3460,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Responding</t>
+          <t>Recieving</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -3031,17 +3470,23 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>[('describe', 'Receiving'), ('underlie', 'Verb not mapped')]</t>
+          <t>[('describe', 'Receiving')]</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>[('allow', 'Responding'), ('relay', 'Responding'), ('follow', 'Receiving'), ('guide', 'Valuing'), ('justify', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Describe into the need for sound data, information and technology governance strategies;</t>
+          <t xml:space="preserve">
+Describe the steps involved in various manufacturing processes for production at scale, including their strengths and limitations.</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3051,7 +3496,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Recieving</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3061,18 +3506,23 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>[('describe', 'Receiving')]</t>
+          <t>[('describe', 'Receiving'), ('involve', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>[('perform', 'Characterisation'), ('identify', 'Receiving'), ('adopt', 'Valuing'), ('support', 'Valuing'), ('allow', 'Responding')]</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Explain the alignment of an organisation's IT strategy, platforms and systems with the overall organisational strategy and management functions</t>
+Select appropriate part manufacturing processes while balancing functional requirements, performance, cost and sustainability.</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3082,28 +3532,33 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Valuing, organisation</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Valuing</t>
+          <t>Receiving</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>[('explain', 'Valuing')]</t>
+          <t>[('select', 'Receiving'), ('balance', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>[('act', 'Characterisation'), ('change', 'Characterisation'), ('present', 'Responding'), ('monitor', 'Valuing'), ('query', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Describe the steps involved in various manufacturing processes for production at scale, including their strengths and limitations.</t>
+Identify and carry out the necessary steps to conduct a small-scale production run and then reflect on the outcomes.</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3123,18 +3578,23 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>[('describe', 'Receiving'), ('involve', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+          <t>[('identify', 'Receiving'), ('carry', 'Verb not mapped'), ('conduct', 'Verb not mapped'), ('reflect', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>[('contribute', 'Valuing'), ('guide', 'Valuing'), ('respond', 'Responding'), ('synthesise', 'Organisation'), ('allow', 'Responding')]</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Select appropriate part manufacturing processes while balancing functional requirements, performance, cost and sustainability.</t>
+Evaluate the functionality and performance of these programs using software development tools.</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3144,7 +3604,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Responding</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3154,18 +3614,23 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>[('select', 'Receiving'), ('balance', 'Verb not mapped')]</t>
+          <t>[('evaluate', 'Valuing'), ('use', 'Receiving')]</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>[('describe', 'Receiving'), ('guide', 'Valuing'), ('organise', 'Organisation'), ('allow', 'Responding'), ('justify', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Identify and carry out the necessary steps to conduct a small-scale production run and then reflect on the outcomes.</t>
+Describe the operation of computer arithmetic, assemblers and compilers, a RISC processor datapath and solve related problems.</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3185,18 +3650,22 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>[('identify', 'Receiving'), ('carry', 'Verb not mapped'), ('conduct', 'Verb not mapped'), ('reflect', 'Verb not mapped')]</t>
+          <t>[('describe', 'Receiving'), ('solve', 'Characterisation')]</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>[('practise', 'Characterisation'), ('manage', 'Organisation'), ('design', 'Organisation'), ('propose', 'Characterisation'), ('justify', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Evaluate the functionality and performance of these programs using software development tools.</t>
+          <t>Solve real-world engineering problems by designing ladder logic diagrams for programmable logic controllers (PLC) using components such as normally open contacts, normally closed contacts, relays, timers and counters.</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3206,7 +3675,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Valuing</t>
+          <t>Characterisation</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3216,18 +3685,23 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>[('evaluate', 'Valuing'), ('use', 'Receiving')]</t>
+          <t>[('solve', 'Characterisation'), ('design', 'Organisation'), ('use', 'Receiving')]</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>[('describe', 'Receiving'), ('guide', 'Valuing'), ('organise', 'Organisation'), ('allow', 'Responding'), ('justify', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Describe the operation of computer arithmetic, assemblers and compilers, a RISC processor datapath and solve related problems.</t>
+Evaluate the various NDT methods for flaw detection and damage assessment and be able to identify the appropriate technique for a given scenario.</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3237,7 +3711,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Responding</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3247,17 +3721,22 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>[('describe', 'Receiving'), ('solve', 'Characterisation')]</t>
+          <t>[('evaluate', 'Valuing'), ('identify', 'Receiving'), ('give', 'Receiving')]</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>[('justify', 'Valuing'), ('change', 'Characterisation'), ('select', 'Receiving'), ('prepare', 'Organisation'), ('respond', 'Responding')]</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Solve real-world engineering problems by designing ladder logic diagrams for programmable logic controllers (PLC) using components such as normally open contacts, normally closed contacts, relays, timers and counters.</t>
+          <t>Solve engineering problems related to design and operation of bioreactors.</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3267,28 +3746,32 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Characterisation, Organization</t>
+          <t>Characterisation</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Receiving</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>[('solve', 'Characterisation'), ('design', 'Organisation'), ('use', 'Receiving')]</t>
+          <t>[('solve', 'Characterisation'), ('relate', 'Organisation')]</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>[('change', 'Characterisation'), ('establish', 'Organisation'), ('investigate', 'Organisation'), ('delay', 'Valuing'), ('allow', 'Responding')]</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Relate the capabilities and limitations of established NDT techniques to their respective basic working principles.</t>
+          <t>Operate bioreactor and evaluate the performance of cell growth under different operating conditions.</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3298,28 +3781,33 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>[('relate', 'Organisation'), ('establish', 'Organisation')]</t>
+          <t>[('operate', 'Verb not mapped'), ('evaluate', 'Valuing')]</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>[('perform', 'Characterisation'), ('present', 'Responding'), ('agree', 'Responding'), ('allow', 'Responding'), ('delay', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Evaluate the various NDT methods for flaw detection and damage assessment and be able to identify the appropriate technique for a given scenario.</t>
+Simulate cameras using projective and multi-view geometry to design model-based vision systems and algorithms that extract 3D and rotational information from images, alongside methods for image registration and stitching.</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3329,7 +3817,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Valuing, Responding</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3339,17 +3827,23 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>[('evaluate', 'Valuing'), ('identify', 'Receiving'), ('give', 'Receiving')]</t>
+          <t>[('simulate', 'Verb not mapped'), ('use', 'Receiving'), ('design', 'Organisation'), ('base', 'Verb not mapped'), ('extract', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>[('guide', 'Valuing'), ('act', 'Characterisation'), ('integrate', 'Organisation'), ('write', 'Responding'), ('agree', 'Responding')]</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Relate bioprocess organisms and their nutrient requirement to bioprocess considerations.</t>
+          <t xml:space="preserve">
+Demonstrate the development, training and deployment of computer vision algorithms using a high-level programming language.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3359,27 +3853,33 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Receiving</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>[('relate', 'Organisation')]</t>
+          <t>[('demonstrate', 'Valuing'), ('use', 'Receiving')]</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>[('describe', 'Receiving'), ('guide', 'Valuing'), ('organise', 'Organisation'), ('allow', 'Responding'), ('justify', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Solve engineering problems related to design and operation of bioreactors.</t>
+          <t xml:space="preserve">
+Identify the limits of human visual and aural perception, and how they can be exploited for bit rate reduction.</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3389,27 +3889,33 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Characterisation</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Receiving</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>[('solve', 'Characterisation'), ('relate', 'Organisation')]</t>
+          <t>[('identify', 'Receiving'), ('exploit', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>[('agree', 'Responding'), ('act', 'Characterisation'), ('perform', 'Characterisation'), ('delay', 'Valuing'), ('allow', 'Responding')]</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Operate bioreactor and evaluate the performance of cell growth under different operating conditions.</t>
+          <t xml:space="preserve">
+Describe the structure of modern multimedia compression systems, and how they exploit the characteristics of both the media itself and human consumers of the media.</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3419,28 +3925,32 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Responding, Valuing</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Valuing</t>
+          <t>Receiving</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>[('operate', 'Verb not mapped'), ('evaluate', 'Valuing')]</t>
+          <t>[('describe', 'Receiving'), ('exploit', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>[('agree', 'Responding'), ('act', 'Characterisation'), ('perform', 'Characterisation'), ('delay', 'Valuing'), ('allow', 'Responding')]</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Simulate cameras using projective and multi-view geometry to design model-based vision systems and algorithms that extract 3D and rotational information from images, alongside methods for image registration and stitching.</t>
+          <t>Compute the end-to-end delay performance of modern Internet protocols supporting media streaming, and relate this to service requirements for on-demand and communicative multimedia services.</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3450,27 +3960,33 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Receiving</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>[('simulate', 'Verb not mapped'), ('use', 'Receiving'), ('design', 'Organisation'), ('base', 'Verb not mapped'), ('extract', 'Verb not mapped')]</t>
+          <t>[('compute', 'Verb not mapped'), ('support', 'Valuing'), ('relate', 'Organisation')]</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>[('change', 'Characterisation'), ('establish', 'Organisation'), ('investigate', 'Organisation'), ('delay', 'Valuing'), ('allow', 'Responding')]</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Design ethical machine learning solutions to problems in computer vision, such as image classification, 3D reconstruction and pose estimation, object detection and semantic segmentation, by critically appraising information and publications.</t>
+          <t xml:space="preserve">
+Describe concepts and fundamentals of deep learning, such as the backpropagation algorithm and adversarial learning.</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3480,28 +3996,33 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Receiving</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>[('design', 'Organisation'), ('appraise', 'Verb not mapped')]</t>
+          <t>[('describe', 'Receiving')]</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>[('allow', 'Responding'), ('relay', 'Responding'), ('follow', 'Receiving'), ('guide', 'Valuing'), ('justify', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Demonstrate the development, training and deployment of computer vision algorithms using a high-level programming language.</t>
+Demonstrate the training and deployment of neural networks using a high level programming language.</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3522,17 +4043,22 @@
       <c r="F105" t="inlineStr">
         <is>
           <t>[('demonstrate', 'Valuing'), ('use', 'Receiving')]</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>[('describe', 'Receiving'), ('guide', 'Valuing'), ('organise', 'Organisation'), ('allow', 'Responding'), ('justify', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Identify the limits of human visual and aural perception, and how they can be exploited for bit rate reduction.</t>
+Appraise critically the sources of information and contents of scientific publications and choose relevant information.</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3552,18 +4078,23 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>[('identify', 'Receiving'), ('exploit', 'Verb not mapped')]</t>
+          <t>[('appraise', 'Verb not mapped'), ('choose', 'Receiving')]</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>[('adopt', 'Valuing'), ('respond', 'Responding'), ('act', 'Characterisation'), ('allow', 'Responding'), ('perform', 'Characterisation')]</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Describe the structure of modern multimedia compression systems, and how they exploit the characteristics of both the media itself and human consumers of the media.</t>
+Select suitable electronic components and develop simple MEMS or Organic electronic device based systems, evaluate structural and material properties of Micro/Nano devices through simulation studies</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3583,17 +4114,23 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>[('describe', 'Receiving'), ('exploit', 'Verb not mapped')]</t>
+          <t>[('select', 'Receiving'), ('develop', 'Verb not mapped'), ('base', 'Verb not mapped'), ('evaluate', 'Valuing')]</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>[('perform', 'Characterisation'), ('present', 'Responding'), ('agree', 'Responding'), ('allow', 'Responding'), ('delay', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Compute the end-to-end delay performance of modern Internet protocols supporting media streaming, and relate this to service requirements for on-demand and communicative multimedia services.</t>
+          <t xml:space="preserve">
+Summarise fundamentals of nanotechnology and propose research opportunities in designing Micro technologies</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3603,1757 +4140,58 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Organization</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Valuing</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>[('compute', 'Verb not mapped'), ('support', 'Valuing'), ('relate', 'Organisation')]</t>
+          <t>[('summarise', 'Verb not mapped'), ('propose', 'Characterisation'), ('design', 'Organisation')]</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>[('select', 'Receiving'), ('solve', 'Characterisation'), ('propose', 'Characterisation'), ('design', 'Organisation'), ('justify', 'Valuing')]</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B109" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-As part of a team, research and investigate an area of interest beyond lecture material, involving software simulations and analysis of results.</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Affective</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>Organization</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>Organisation</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>[('research', 'Verb not mapped'), ('investigate', 'Organisation'), ('involve', 'Verb not mapped')]</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>169</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Describe concepts and fundamentals of deep learning, such as the backpropagation algorithm and adversarial learning.</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>Affective</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>Responding</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>Receiving</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>[('describe', 'Receiving')]</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>172</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Design deep learning solutions to problems in computer vision, natural language processing and signal processing. Examples are image classification, object detection, sequence modelling and filter design.</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>Affective</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>Organization</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>Organisation</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>[('design', 'Organisation')]</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>173</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Demonstrate the training and deployment of neural networks using a high level programming language.</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>Affective</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Responding</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>Receiving</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>[('demonstrate', 'Valuing'), ('use', 'Receiving')]</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>174</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Appraise critically the sources of information and contents of scientific publications and choose relevant information.</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Affective</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Responding</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>Receiving</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>[('appraise', 'Verb not mapped'), ('choose', 'Receiving')]</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>176</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Design and develop simple MEMS devices, organic electronic devices (such as Organic Light Emitting Diode) and theoretical models involving multi physics</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>Affective</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>Organization</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>Organisation</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>[('design', 'Organisation'), ('develop', 'Verb not mapped'), ('involve', 'Verb not mapped')]</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>177</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Select suitable electronic components and develop simple MEMS or Organic electronic device based systems, evaluate structural and material properties of Micro/Nano devices through simulation studies</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>Affective</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>Responding, Valuing</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>Receiving</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>[('select', 'Receiving'), ('develop', 'Verb not mapped'), ('base', 'Verb not mapped'), ('evaluate', 'Valuing')]</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>178</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Summarise fundamentals of nanotechnology and propose research opportunities in designing Micro technologies</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>Affective</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>Valuing</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>Organisation</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>[('summarise', 'Verb not mapped'), ('propose', 'Characterisation'), ('design', 'Organisation')]</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>181</v>
-      </c>
-      <c r="B117" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Design and implement a system to solve a given complex engineering problem in the field of Intelligent lighting control using the knowledge of SSL.</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Affective</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>Organization</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Organisation</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
         <is>
           <t>Receiving</t>
         </is>
       </c>
-      <c r="F117" t="inlineStr">
+      <c r="F109" t="inlineStr">
         <is>
           <t>[('design', 'Organisation'), ('implement', 'Verb not mapped'), ('solve', 'Characterisation'), ('give', 'Receiving'), ('use', 'Receiving')]</t>
         </is>
       </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>182</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Conduct experiments to investigate various relationships in photometry, radiometry, colour quality, the energy consumption of light sources and the implementation of IoT-based lighting control.</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>Affective</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>Organization</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>Organisation</t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>[('conduct', 'Verb not mapped'), ('investigate', 'Organisation'), ('base', 'Verb not mapped')]</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B118"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Suggested Verbs</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>84</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>86</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>95</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>97</v>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>98</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>106</v>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>116</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>117</v>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>118</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>122</v>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>123</v>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="n">
-        <v>124</v>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="n">
-        <v>127</v>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="n">
-        <v>128</v>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="n">
-        <v>129</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="n">
-        <v>130</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="n">
-        <v>131</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="n">
-        <v>132</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="n">
-        <v>135</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>137</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="n">
-        <v>138</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>139</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>141</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="n">
-        <v>144</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>145</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>146</v>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="n">
-        <v>148</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>149</v>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>152</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>153</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>155</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>158</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>161</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>162</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>163</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>164</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>166</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>168</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>169</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>172</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>173</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>174</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>176</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>177</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>178</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>181</v>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>182</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>Empty DataFrame
-Columns: [Level]
-Index: []</t>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>[('describe', 'Receiving'), ('guide', 'Valuing'), ('organise', 'Organisation'), ('allow', 'Responding'), ('justify', 'Valuing')]</t>
         </is>
       </c>
     </row>

</xml_diff>